<commit_message>
Commit via Qualitia by veronica
</commit_message>
<xml_diff>
--- a/Demo1_projectdb/TestCases/Signup.xlsx
+++ b/Demo1_projectdb/TestCases/Signup.xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
-    <t>$NULL$</t>
-  </si>
-  <si>
     <t>TC001</t>
   </si>
   <si>
@@ -32,6 +29,9 @@
   </si>
   <si>
     <t>TCIteration</t>
+  </si>
+  <si>
+    <t>abc@gmai.com</t>
   </si>
 </sst>
 </file>
@@ -728,23 +728,23 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="16"/>
     </row>
     <row r="2" ht="25" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>4</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="16"/>
@@ -758,7 +758,7 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="15" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F3" s="14"/>
     </row>

</xml_diff>